<commit_message>
Add timesheets week 8 and 9
</commit_message>
<xml_diff>
--- a/Admin/Filip/TimeSheet_Week8.xlsx
+++ b/Admin/Filip/TimeSheet_Week8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\OneDrive\Documents\Capstone\SeniorDesignProject\Admin\Filip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FF16A2-3785-44B7-896B-C9345CC06BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3C75A6-C99D-4697-8006-87207DA9C96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,10 +761,12 @@
         <v>2</v>
       </c>
       <c r="G8" s="10"/>
-      <c r="H8" s="9"/>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
       <c r="I8" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J8" s="7"/>
     </row>
@@ -870,11 +872,11 @@
       </c>
       <c r="H13" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="11">
         <f>SUM(I6:I12)</f>
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>